<commit_message>
2. Lab2: add models
</commit_message>
<xml_diff>
--- a/requirements/user_stories.xlsx
+++ b/requirements/user_stories.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,13 +11,123 @@
     <sheet name="Аркуш2" sheetId="2" r:id="rId2"/>
     <sheet name="Аркуш3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Importance</t>
+  </si>
+  <si>
+    <t>Initial estimate</t>
+  </si>
+  <si>
+    <t>How to demo</t>
+  </si>
+  <si>
+    <t>Acceptance criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сотрудник отдела маркетинга должен </t>
+  </si>
+  <si>
+    <t xml:space="preserve">просматривать информацию о наличиипродукции </t>
+  </si>
+  <si>
+    <t>на складе, чтобі обработать заказ клиента</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сотрудник отдела маркетинга должен работать </t>
+  </si>
+  <si>
+    <t xml:space="preserve">с информацией о поставщиках, чтобі сформировать </t>
+  </si>
+  <si>
+    <t>заказ на поставку</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сотрудник отдела снабжения должен работать с </t>
+  </si>
+  <si>
+    <t>информацией о договорах чтобі зарегестрировать в</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> системе заключение договора на поставку </t>
+  </si>
+  <si>
+    <t xml:space="preserve">информацией о поставленых товарах , чтобы обновить </t>
+  </si>
+  <si>
+    <t>данные о наличии продукции на складе</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сотрудник отдела снабжения должен формировать </t>
+  </si>
+  <si>
+    <t>приходную накладную, чтобы оформить приход товара на склад</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сотрудник отдела бухгалтерии должен формировать </t>
+  </si>
+  <si>
+    <t>счет на оплату, чтобы оплатить поставку</t>
+  </si>
+  <si>
+    <t>returnListOfAvProd()</t>
+  </si>
+  <si>
+    <t>returnPurchInvoice()</t>
+  </si>
+  <si>
+    <t>returnPayInvoice()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">createLESup(), create PESup(), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">updateLESup(), updatePESup(), </t>
+  </si>
+  <si>
+    <t>removeSup(), returnSup()</t>
+  </si>
+  <si>
+    <t>remaveContract(), returnListContract()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">createContract(), updateContract(), </t>
+  </si>
+  <si>
+    <t>createSupProd(), updateSupProd(),</t>
+  </si>
+  <si>
+    <t>remaveSupProd(),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>returnListSupProdByContNum()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Успешное </t>
+  </si>
+  <si>
+    <t>прохождениетеста</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -26,15 +136,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -42,25 +158,120 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартна">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -98,7 +309,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартна">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -170,7 +381,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартна">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -343,36 +554,313 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="51.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>